<commit_message>
Update text labels and LiveChat license in various components for consistency and clarity
</commit_message>
<xml_diff>
--- a/Client/src/pages/admin/warehouse/data/template.xlsx
+++ b/Client/src/pages/admin/warehouse/data/template.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Warehouse Import Template" sheetId="1" r:id="rId4"/>
+    <sheet name="Warehouse Import Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="151">
   <si>
     <t>ingredientName</t>
   </si>
@@ -40,183 +56,1340 @@
     <t>categoryName</t>
   </si>
   <si>
-    <t>sticky rices</t>
+    <t>Beef</t>
   </si>
   <si>
     <t>kilogram</t>
   </si>
   <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
-    <t>2024-10-30</t>
-  </si>
-  <si>
-    <t>sticky rices grade 1</t>
-  </si>
-  <si>
-    <t>Tap hoa Trang Phuong</t>
-  </si>
-  <si>
-    <t>f8e6ab5c-c87d-4c8c-b2f6-0ca5bb8836ac</t>
-  </si>
-  <si>
-    <t>jasmine rice</t>
-  </si>
-  <si>
-    <t>2024-10-01</t>
-  </si>
-  <si>
-    <t>2024-10-31</t>
-  </si>
-  <si>
-    <t>jasmine rice grade 1</t>
-  </si>
-  <si>
-    <t>Nha Trang Rice Co.</t>
-  </si>
-  <si>
-    <t>brown rice</t>
-  </si>
-  <si>
-    <t>2024-10-02</t>
-  </si>
-  <si>
-    <t>2024-11-01</t>
-  </si>
-  <si>
-    <t>brown rice organic</t>
-  </si>
-  <si>
-    <t>Organic Food Corp.</t>
-  </si>
-  <si>
-    <t>quinoa</t>
-  </si>
-  <si>
-    <t>2024-10-03</t>
-  </si>
-  <si>
-    <t>2024-11-02</t>
-  </si>
-  <si>
-    <t>quinoa high protein</t>
-  </si>
-  <si>
-    <t>Super Grains Inc.</t>
-  </si>
-  <si>
-    <t>red rice</t>
-  </si>
-  <si>
-    <t>2024-10-04</t>
-  </si>
-  <si>
-    <t>2024-11-03</t>
-  </si>
-  <si>
-    <t>red rice traditional</t>
-  </si>
-  <si>
-    <t>Traditional Rice Supplies</t>
+    <t>2024-09-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2025-02-30 00:00:00</t>
+  </si>
+  <si>
+    <t>Grade A beef</t>
+  </si>
+  <si>
+    <t>Grocery Thanh Binh</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Fresh pork</t>
+  </si>
+  <si>
+    <t>Thit Heo Phuong Dong</t>
+  </si>
+  <si>
+    <t>Pork chop</t>
+  </si>
+  <si>
+    <t>Pork chops</t>
+  </si>
+  <si>
+    <t>Grocery Huong Tra</t>
+  </si>
+  <si>
+    <t>Pork belly</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Fresh chicken</t>
+  </si>
+  <si>
+    <t>Grocery Minh Tam</t>
+  </si>
+  <si>
+    <t>Poultry</t>
+  </si>
+  <si>
+    <t>Quail eggs</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>Organic quail eggs</t>
+  </si>
+  <si>
+    <t>Shrimp</t>
+  </si>
+  <si>
+    <t>Fresh shrimp</t>
+  </si>
+  <si>
+    <t>Hai San Bien Dong</t>
+  </si>
+  <si>
+    <t>Seafood</t>
+  </si>
+  <si>
+    <t>Fish fillet</t>
+  </si>
+  <si>
+    <t>Clams</t>
+  </si>
+  <si>
+    <t>Fresh clams</t>
+  </si>
+  <si>
+    <t>Hai San Tuoi Song</t>
+  </si>
+  <si>
+    <t>Snakehead fish</t>
+  </si>
+  <si>
+    <t>Cilantro</t>
+  </si>
+  <si>
+    <t>Fresh cilantro</t>
+  </si>
+  <si>
+    <t>Grocery Xanh</t>
+  </si>
+  <si>
+    <t>Herbs</t>
+  </si>
+  <si>
+    <t>Green onions</t>
+  </si>
+  <si>
+    <t>Fresh green onions</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
+  </si>
+  <si>
+    <t>Fresh lettuce</t>
+  </si>
+  <si>
+    <t>Greens &amp; Vegetables</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>Fresh cucumber</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Organic carrot</t>
+  </si>
+  <si>
+    <t>Rau Cu Sach Thanh Hang</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Ripe tomato</t>
+  </si>
+  <si>
+    <t>Taro stem</t>
+  </si>
+  <si>
+    <t>Fresh taro stem</t>
+  </si>
+  <si>
+    <t>Bean sprouts</t>
+  </si>
+  <si>
+    <t>Fresh bean sprouts</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Sea salt</t>
+  </si>
+  <si>
+    <t>Basic Seasonings</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Black pepper</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Granulated sugar</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Fresh garlic</t>
+  </si>
+  <si>
+    <t>Shallots</t>
+  </si>
+  <si>
+    <t>Fresh shallots</t>
+  </si>
+  <si>
+    <t>Lime</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>Fresh lime juice</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Fresh ginger</t>
+  </si>
+  <si>
+    <t>Special Seasonings</t>
+  </si>
+  <si>
+    <t>Star anise</t>
+  </si>
+  <si>
+    <t>Star anise spice</t>
+  </si>
+  <si>
+    <t>Cinnamon</t>
+  </si>
+  <si>
+    <t>Ceylon cinnamon stick</t>
+  </si>
+  <si>
+    <t>Turmeric</t>
+  </si>
+  <si>
+    <t>Ground turmeric</t>
+  </si>
+  <si>
+    <t>Annatto oil</t>
+  </si>
+  <si>
+    <t>Lemongrass</t>
+  </si>
+  <si>
+    <t>Fresh lemongrass</t>
+  </si>
+  <si>
+    <t>Chili</t>
+  </si>
+  <si>
+    <t>Fresh chili</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Baguette</t>
+  </si>
+  <si>
+    <t>Fresh baguette</t>
+  </si>
+  <si>
+    <t>Grocery Trang Phuong</t>
+  </si>
+  <si>
+    <t>Noodles &amp; Rice</t>
+  </si>
+  <si>
+    <t>Pho noodles</t>
+  </si>
+  <si>
+    <t>Rice pho noodles</t>
+  </si>
+  <si>
+    <t>Nha May Mi Dai Cuong</t>
+  </si>
+  <si>
+    <t>Rice vermicelli</t>
+  </si>
+  <si>
+    <t>Quang noodles</t>
+  </si>
+  <si>
+    <t>Vermicelli noodles</t>
+  </si>
+  <si>
+    <t>Thin vermicelli noodles</t>
+  </si>
+  <si>
+    <t>Rice &amp; Flour</t>
+  </si>
+  <si>
+    <t>Broken rice</t>
+  </si>
+  <si>
+    <t>Broken rice grains</t>
+  </si>
+  <si>
+    <t>Rice flour</t>
+  </si>
+  <si>
+    <t>Rice flour for rolls</t>
+  </si>
+  <si>
+    <t>Broths</t>
+  </si>
+  <si>
+    <t>Beef broth</t>
+  </si>
+  <si>
+    <t>Beef bone broth</t>
+  </si>
+  <si>
+    <t>Chicken broth</t>
+  </si>
+  <si>
+    <t>Chicken bone broth</t>
+  </si>
+  <si>
+    <t>Thai hot pot broth</t>
+  </si>
+  <si>
+    <t>Sauces</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>General purpose sauce</t>
+  </si>
+  <si>
+    <t>Sweet fish sauce</t>
+  </si>
+  <si>
+    <t>Fish sauce</t>
+  </si>
+  <si>
+    <t>Pure fish sauce</t>
+  </si>
+  <si>
+    <t>Dipping sauce</t>
+  </si>
+  <si>
+    <t>Dipping sauce for rolls</t>
+  </si>
+  <si>
+    <t>Eggs &amp; Miscellaneous</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Fresh egg</t>
+  </si>
+  <si>
+    <t>Additional Ingredients</t>
+  </si>
+  <si>
+    <t>Rice crackers</t>
+  </si>
+  <si>
+    <t>Crispy rice crackers</t>
+  </si>
+  <si>
+    <t>Wood ear mushroom</t>
+  </si>
+  <si>
+    <t>Wood ear mushrooms</t>
+  </si>
+  <si>
+    <t>Fried shallots</t>
+  </si>
+  <si>
+    <t>Crispy fried shallots</t>
+  </si>
+  <si>
+    <t>Crushed peanuts</t>
+  </si>
+  <si>
+    <t>Cooking oil</t>
+  </si>
+  <si>
+    <t>Pure vegetable oil</t>
+  </si>
+  <si>
+    <t>Tiger shrimp</t>
+  </si>
+  <si>
+    <t>Fresh tiger shrimp</t>
+  </si>
+  <si>
+    <t>Squid</t>
+  </si>
+  <si>
+    <t>Fresh squid</t>
+  </si>
+  <si>
+    <t>Mushrooms</t>
+  </si>
+  <si>
+    <t>Mixed fresh mushrooms</t>
+  </si>
+  <si>
+    <t>Water spinach</t>
+  </si>
+  <si>
+    <t>Fresh water spinach</t>
+  </si>
+  <si>
+    <t>Basil leaves</t>
+  </si>
+  <si>
+    <t>Fresh basil leaves</t>
+  </si>
+  <si>
+    <t>Fermented tofu</t>
+  </si>
+  <si>
+    <t>Soft fermented tofu</t>
+  </si>
+  <si>
+    <t>Lobster</t>
+  </si>
+  <si>
+    <t>Fresh lobster</t>
+  </si>
+  <si>
+    <t>Tamarind</t>
+  </si>
+  <si>
+    <t>Tamarind pulp</t>
+  </si>
+  <si>
+    <t>Passion fruit</t>
+  </si>
+  <si>
+    <t>Fresh passion fruit</t>
+  </si>
+  <si>
+    <t>Lamb chops</t>
+  </si>
+  <si>
+    <t>Fresh lamb chops</t>
+  </si>
+  <si>
+    <t>Meat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -406,249 +1579,1830 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.29"/>
-    <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="3" max="3" width="14.29"/>
-    <col customWidth="1" min="4" max="5" width="23.43"/>
-    <col customWidth="1" min="6" max="6" width="20.29"/>
-    <col customWidth="1" min="7" max="7" width="18.57"/>
-    <col customWidth="1" min="8" max="8" width="26.43"/>
-    <col customWidth="1" min="9" max="9" width="39.57"/>
-    <col customWidth="1" min="10" max="26" width="8.71"/>
+    <col min="1" max="1" width="23.287037037037" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="14.287037037037" customWidth="1"/>
+    <col min="4" max="5" width="23.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="20.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="18.5740740740741" customWidth="1"/>
+    <col min="8" max="8" width="26.4259259259259" customWidth="1"/>
+    <col min="9" max="9" width="39.5740740740741" customWidth="1"/>
+    <col min="10" max="26" width="8.71296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.4" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="14.4" spans="1:9">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3">
-        <v>11300.0</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="B2" s="2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4">
+        <v>180000</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" ht="14.4" spans="1:9">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4">
+        <v>130000</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3">
-        <v>200.0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" ht="14.4" spans="1:9">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="B4" s="2">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4">
+        <v>150000</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="5" ht="14.4" spans="1:9">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3">
-        <v>150.0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="B5" s="2">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
+        <v>140000</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="14.4" spans="1:9">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="B6" s="2">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4">
+        <v>90000</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3">
-        <v>11500.0</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="4" t="s">
+    </row>
+    <row r="7" ht="14.4" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4">
+        <v>230000</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2">
+        <v>100</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4">
+        <v>180000</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2">
+        <v>200</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4">
+        <v>160000</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:9">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4">
+        <v>40000</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:9">
+      <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4">
+        <v>25000</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3">
-        <v>50.0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="4">
+        <v>20000</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:9">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="4">
+        <v>25000</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:9">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4">
+        <v>18000</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:9">
+      <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="4">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:9">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:9">
+      <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="4">
+        <v>200000</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4">
+        <v>30000</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="4">
+        <v>35000</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5000</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="2">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="4">
+        <v>35000</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3">
-        <v>15000.0</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="4">
+        <v>100</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="4">
+        <v>45000</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4">
+        <v>45000</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="2">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="4">
+        <v>25000</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="2">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="4">
+        <v>60000</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2">
+        <v>50</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4">
+        <v>3000</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="2">
+        <v>150</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="4">
+        <v>40000</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="2">
+        <v>200</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="4">
+        <v>35000</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="2">
+        <v>200</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="4">
+        <v>50000</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="2">
+        <v>20</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="4">
+        <v>40000</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="2">
+        <v>200</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="2">
+        <v>100</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="4">
+        <v>20000</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="2">
+        <v>400</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="4">
+        <v>60000</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="2">
+        <v>300</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="4">
+        <v>55000</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="2">
+        <v>400</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="4">
+        <v>70000</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="2">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="2">
+        <v>20</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="2">
+        <v>20</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="2">
+        <v>15</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="2">
+        <v>50</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="4">
+        <v>3000</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A48" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="2">
+        <v>50</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="4">
+        <v>5000</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A49" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="2">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="4">
+        <v>80000</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A50" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="2">
+        <v>10</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="4">
+        <v>45000</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A51" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="2">
+        <v>10</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="4">
+        <v>40000</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A52" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="2">
+        <v>20</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="4">
+        <v>30000</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A53" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="2">
         <v>30</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="C53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="4">
+        <v>230000</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="2">
+        <v>20</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="4">
+        <v>210000</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A55" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="2">
+        <v>10</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="4">
+        <v>80000</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A56" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="4">
+        <v>20000</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A57" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="2">
+        <v>10</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="4">
+        <v>50000</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A58" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B58" s="2">
+        <v>10</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="4">
+        <v>60000</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A59" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="2">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="4">
+        <v>450000</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3">
-        <v>75.0</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="I59" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3">
-        <v>14000.0</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="6"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A60" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="2">
+        <v>5</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="4">
+        <v>70000</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A61" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="2">
+        <v>5</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="4">
+        <v>40000</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A62" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="2">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="4">
+        <v>400000</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
@@ -1586,11 +4340,9 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>